<commit_message>
Folders for level waves
</commit_message>
<xml_diff>
--- a/Assets/Scripts/GameManager/DataManagement/WaveSystemTemplate.xlsx
+++ b/Assets/Scripts/GameManager/DataManagement/WaveSystemTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhelm\Desktop\TC\BuggerOff-_Mobile\Assets\Scripts\GameManager\DataManagement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Veikka\Documents\GitHub\BuggerOff-_Mobile\Assets\Scripts\GameManager\DataManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5509A807-14DD-4730-B843-E68CDF985D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DBFC43-1168-45AF-A8A4-E9AD02BBEB81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1407F9EC-89FA-41FB-A318-2CEEB923D5FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1407F9EC-89FA-41FB-A318-2CEEB923D5FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -402,12 +402,12 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>